<commit_message>
* Implements threading to control the timing * Add todo in the code * Update performance tests
</commit_message>
<xml_diff>
--- a/Documents/testPerformance.xlsx
+++ b/Documents/testPerformance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="100" windowWidth="21600" windowHeight="14600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13380" yWindow="100" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1557,6 +1557,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1570,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1986,6 +1987,16 @@
         <f>AVERAGE(G34:G38)</f>
         <v>5110.3999999999996</v>
       </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
* Add README with listing * Add minor refactorisation * FOUND BUG : it doesn't work with PVC tester (allways returns the first value processed)
</commit_message>
<xml_diff>
--- a/Documents/testPerformance.xlsx
+++ b/Documents/testPerformance.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="100" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11520" yWindow="2700" windowWidth="21600" windowHeight="14660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Optimisations" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,94 +21,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="24">
   <si>
     <t>routesNumber</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pe1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pe2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>epsilon</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>essai1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>length</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>I</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>N</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>T</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Q</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>U</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>paramètres standards:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>OPTIMISATION 1: utiliser routelen au lieu d'un appel de méthode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> + OPTIMISATION 2: utilisation des slots</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> + OPTIMISATION 3: optimisation de l'inversion (m2)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> + OPTIMISATION 3: optimisation de l'inversion (m1)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> + OPTIMISATION 4 : </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fonction eval:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fonction route</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fonction cities puis route</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -141,8 +163,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1557,10 +1580,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1573,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1988,6 +2009,11 @@
         <v>5110.3999999999996</v>
       </c>
     </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="48" spans="1:7">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1999,7 +2025,209 @@
       <c r="C55" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>2853</v>
+      </c>
+      <c r="C10">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2906</v>
+      </c>
+      <c r="C11">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2820</v>
+      </c>
+      <c r="C12">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2941</v>
+      </c>
+      <c r="C13">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2862</v>
+      </c>
+      <c r="C14">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="1">
+        <f>AVERAGE(B10:B14)</f>
+        <v>2876.4</v>
+      </c>
+      <c r="C15" s="1">
+        <f>AVERAGE(C10:C14)</f>
+        <v>2243.1999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>2846</v>
+      </c>
+      <c r="C20">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>2829</v>
+      </c>
+      <c r="C21">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="1">
+        <f>AVERAGE(B20:B24)</f>
+        <v>2837.5</v>
+      </c>
+      <c r="C25" s="1">
+        <f>AVERAGE(C20:C24)</f>
+        <v>2305</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>